<commit_message>
Updated config2 file and included the catch exception of assert error for share set, comparison and exploration fail
</commit_message>
<xml_diff>
--- a/Resources/Configuration2.xlsx
+++ b/Resources/Configuration2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4808B1DB-5402-4028-B372-38F977EF4914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18557AC7-AEA7-4355-AAC5-2D6D6B86A5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -348,9 +348,6 @@
     <t>&lt;Set Name to be created&gt;,&lt;entity to be selected&gt;,&lt;search text for creating set&gt;, &lt;No of rows to be set&gt;, &lt;Primary column to be set&gt;, &lt;Secondary column to be set&gt;</t>
   </si>
   <si>
-    <t>GridSet, Disease, Kera, 10, Definition, Identifier</t>
-  </si>
-  <si>
     <t>Create_And_Delete_Set</t>
   </si>
   <si>
@@ -1122,22 +1119,25 @@
     <t>Filter type can only be "contains" or "equals" and filter column refers to the attribute name</t>
   </si>
   <si>
-    <t>Set From File 1,Disease, C:\Users\eagleqateam\Documents\GitHub\SeleniumAutomation\Resources\Q4 - Upload file - 1 (2).xlsx</t>
-  </si>
-  <si>
-    <t>ESFile 1,Disease,kera,Disease, C:\Users\eagleqateam\Documents\GitHub\SeleniumAutomation\Resources\Q4 - Upload file - 1 (2).xlsx, Q4 - Upload file - 1 (2).xlsx</t>
-  </si>
-  <si>
-    <t>ExFileUpload, Disease, C:\Users\eagleqateam\Documents\GitHub\SeleniumAutomation\Resources\Q4 - Upload file - 1 (2).xlsx</t>
-  </si>
-  <si>
-    <t>ExpAddfromFile 1,Disease,kera,Disease, C:\Users\eagleqateam\Documents\GitHub\SeleniumAutomation\Resources\Q4 - Upload file - 1 (2).xlsx, Q4 - Upload file - 1 (2).xlsx</t>
-  </si>
-  <si>
-    <t>ComFileUpload, Control Set, Disease, C:\Users\eagleqateam\Documents\GitHub\SeleniumAutomation\Resources\Q4 - Upload file - 1 (2).xlsx</t>
-  </si>
-  <si>
-    <t>ComAddfromFile 1,Control Card, Disease,kera,Disease, C:\Users\eagleqateam\Documents\GitHub\SeleniumAutomation\Resources\Q4 - Upload file - 1 (2).xlsx, Q4 - Upload file - 1 (2).xlsx</t>
+    <t>GridSet, Disease, Kera, 10, EFO ID, Datasource Name</t>
+  </si>
+  <si>
+    <t>Set From File 1,Disease, C:\Users\MugunthRaman\git\EagleAutomation\Resources\Q4 - Upload file - 1 (2).xlsx</t>
+  </si>
+  <si>
+    <t>ESFile 1,Disease,kera,Disease, C:\Users\MugunthRaman\git\EagleAutomation\Resources\Q4 - Upload file - 1 (2).xlsx, Q4 - Upload file - 1 (2).xlsx</t>
+  </si>
+  <si>
+    <t>ExFileUpload, Disease, C:\Users\MugunthRaman\git\EagleAutomation\Resources\Q4 - Upload file - 1 (2).xlsx</t>
+  </si>
+  <si>
+    <t>ExpAddfromFile 1,Disease,kera,Disease, C:\Users\MugunthRaman\git\EagleAutomation\Resources\Q4 - Upload file - 1 (2).xlsx, Q4 - Upload file - 1 (2).xlsx</t>
+  </si>
+  <si>
+    <t>ComFileUpload, Control Set, Disease, C:\Users\MugunthRaman\git\EagleAutomation\Resources\Q4 - Upload file - 1 (2).xlsx</t>
+  </si>
+  <si>
+    <t>ComAddfromFile 1,Control Card, Disease,kera,Disease, C:\Users\MugunthRaman\git\EagleAutomation\Resources\Q4 - Upload file - 1 (2).xlsx, Q4 - Upload file - 1 (2).xlsx</t>
   </si>
 </sst>
 </file>
@@ -1510,11 +1510,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1634,14 +1634,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B2293B69-6BEF-4876-8041-4E581FDF60A3}" name="Table22" displayName="Table22" ref="A1:E80" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E80" xr:uid="{B2293B69-6BEF-4876-8041-4E581FDF60A3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B767210A-D422-483B-AD7B-C9F9FDA65479}" name="Table223" displayName="Table223" ref="A1:E80" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E80" xr:uid="{B767210A-D422-483B-AD7B-C9F9FDA65479}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{278089CD-41AD-4D0D-A37B-C3F0D49F8E08}" name="Test Case#" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{2B1CEA1A-9C99-4538-BF02-BDB38E61E3CE}" name="FunctionName" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{C6027479-92EE-49EA-B476-5EA7BCF3796C}" name="Description" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{8C627C27-DA49-4E96-9923-45AC6780212C}" name="Parameters" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{75315E8A-E375-4AC6-B082-FB25BA079233}" name="Test Data" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{8D049B3E-72FF-449C-9D1F-12403CA5C52F}" name="Test Case#" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{BD45DD22-295B-40F4-BAC5-F10773ED3F2F}" name="FunctionName" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00395498-2D41-47CE-A1F2-3F17157C1612}" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{2FE7CAE6-6015-4B20-8B6B-E4E732DD62F6}" name="Parameters" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{5AEB2DF3-BA59-4400-9C73-826A6ADF63D3}" name="Test Data" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1947,7 +1947,7 @@
   <dimension ref="A1:H80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,7 +1999,7 @@
       <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="28" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="10"/>
@@ -2298,8 +2298,8 @@
         <v>99</v>
       </c>
       <c r="G18" s="32"/>
-      <c r="H18" s="28" t="s">
-        <v>360</v>
+      <c r="H18" s="27" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2316,61 +2316,61 @@
         <v>103</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>104</v>
+        <v>361</v>
       </c>
       <c r="G19" s="32"/>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G20" s="32"/>
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>113</v>
       </c>
       <c r="G21" s="32"/>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>62</v>
@@ -2380,82 +2380,82 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>122</v>
       </c>
       <c r="G23" s="32"/>
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>127</v>
       </c>
       <c r="G24" s="32"/>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>132</v>
-      </c>
       <c r="G25" s="32"/>
-      <c r="H25" s="28" t="s">
-        <v>361</v>
+      <c r="H25" s="27" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>137</v>
-      </c>
       <c r="G26" s="33"/>
-      <c r="H26" s="28" t="s">
-        <v>361</v>
+      <c r="H26" s="27" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2481,54 +2481,54 @@
     </row>
     <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>142</v>
       </c>
       <c r="G28" s="34"/>
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>145</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>146</v>
       </c>
       <c r="G29" s="34"/>
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>364</v>
@@ -2538,130 +2538,130 @@
     </row>
     <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="6" t="s">
         <v>154</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>155</v>
       </c>
       <c r="G31" s="34"/>
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="G32" s="34"/>
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>163</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="G33" s="34"/>
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>169</v>
       </c>
       <c r="G34" s="34"/>
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>174</v>
       </c>
       <c r="G35" s="34"/>
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="G36" s="34"/>
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>365</v>
@@ -2671,198 +2671,198 @@
     </row>
     <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="G38" s="34"/>
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="G39" s="34"/>
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G40" s="34"/>
       <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="G41" s="34"/>
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>207</v>
       </c>
       <c r="G42" s="34"/>
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="G43" s="34"/>
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>217</v>
-      </c>
       <c r="G44" s="34"/>
-      <c r="H44" s="28" t="s">
-        <v>360</v>
+      <c r="H44" s="27" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>222</v>
       </c>
       <c r="G45" s="34"/>
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="E46" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="E46" s="6" t="s">
-        <v>227</v>
-      </c>
       <c r="G46" s="34"/>
-      <c r="H46" s="28" t="s">
-        <v>361</v>
+      <c r="H46" s="27" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="B47" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="B47" s="23" t="s">
+      <c r="C47" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="C47" s="23" t="s">
+      <c r="D47" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="E47" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="E47" s="25" t="s">
-        <v>232</v>
-      </c>
       <c r="G47" s="35"/>
-      <c r="H47" s="28" t="s">
-        <v>361</v>
+      <c r="H47" s="27" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2888,35 +2888,35 @@
     </row>
     <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="6" t="s">
         <v>236</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>237</v>
       </c>
       <c r="G49" s="34"/>
       <c r="H49" s="10"/>
     </row>
     <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>366</v>
@@ -2926,184 +2926,184 @@
     </row>
     <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="E51" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>246</v>
       </c>
       <c r="G51" s="34"/>
       <c r="H51" s="10"/>
     </row>
     <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E52" s="6" t="s">
         <v>249</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>250</v>
       </c>
       <c r="G52" s="34"/>
       <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="E53" s="6" t="s">
         <v>254</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>255</v>
       </c>
       <c r="G53" s="34"/>
       <c r="H53" s="10"/>
     </row>
     <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="E54" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>260</v>
       </c>
       <c r="G54" s="34"/>
       <c r="H54" s="10"/>
     </row>
     <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" s="6" t="s">
         <v>264</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>265</v>
       </c>
       <c r="G55" s="34"/>
       <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E56" s="6" t="s">
         <v>268</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>269</v>
       </c>
       <c r="G56" s="34"/>
       <c r="H56" s="10"/>
     </row>
     <row r="57" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="E57" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>274</v>
       </c>
       <c r="G57" s="34"/>
       <c r="H57" s="10"/>
     </row>
     <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="6" t="s">
         <v>278</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>279</v>
       </c>
       <c r="G58" s="34"/>
       <c r="H58" s="10"/>
     </row>
     <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="E59" s="6" t="s">
         <v>283</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>284</v>
       </c>
       <c r="G59" s="34"/>
       <c r="H59" s="10"/>
     </row>
     <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>90</v>
@@ -3116,209 +3116,209 @@
     </row>
     <row r="61" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="E61" s="6" t="s">
         <v>291</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>292</v>
       </c>
       <c r="G61" s="34"/>
       <c r="H61" s="10"/>
     </row>
     <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="D62" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>295</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>296</v>
       </c>
       <c r="G62" s="34"/>
       <c r="H62" s="10"/>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="E63" s="6" t="s">
         <v>300</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>301</v>
       </c>
       <c r="G63" s="34"/>
       <c r="H63" s="10"/>
     </row>
     <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="E64" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>306</v>
       </c>
       <c r="G64" s="34"/>
       <c r="H64" s="10"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="E65" s="6" t="s">
         <v>310</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>311</v>
       </c>
       <c r="G65" s="34"/>
       <c r="H65" s="10"/>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="E66" s="6" t="s">
         <v>315</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>316</v>
       </c>
       <c r="G66" s="34"/>
       <c r="H66" s="10"/>
     </row>
     <row r="67" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="E67" s="6" t="s">
         <v>320</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>321</v>
       </c>
       <c r="G67" s="34"/>
       <c r="H67" s="10"/>
     </row>
     <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="E68" s="6" t="s">
         <v>325</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>326</v>
       </c>
       <c r="G68" s="34"/>
       <c r="H68" s="10"/>
     </row>
     <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="E69" s="6" t="s">
         <v>330</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="G69" s="34"/>
       <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="D70" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E70" s="6" t="s">
         <v>334</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>335</v>
       </c>
       <c r="G70" s="34"/>
       <c r="H70" s="10"/>
     </row>
     <row r="71" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="C71" s="23" t="s">
         <v>337</v>
       </c>
-      <c r="C71" s="23" t="s">
+      <c r="D71" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="E71" s="6" t="s">
         <v>338</v>
-      </c>
-      <c r="D71" s="23" t="s">
-        <v>231</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>339</v>
       </c>
       <c r="G71" s="34"/>
       <c r="H71" s="10"/>
@@ -3342,93 +3342,93 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="E73" s="6" t="s">
         <v>341</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>342</v>
       </c>
       <c r="G73" s="30"/>
       <c r="H73" s="10"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="E74" s="6" t="s">
         <v>344</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>345</v>
       </c>
       <c r="G74" s="30"/>
       <c r="H74" s="10"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="E75" s="6" t="s">
         <v>347</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>348</v>
       </c>
       <c r="G75" s="30"/>
       <c r="H75" s="10"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="E76" s="6" t="s">
         <v>350</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>351</v>
       </c>
       <c r="G76" s="30"/>
       <c r="H76" s="10"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="E77" s="6" t="s">
         <v>353</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>354</v>
       </c>
       <c r="G77" s="30"/>
       <c r="H77" s="10"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="E78" s="6" t="s">
         <v>356</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>357</v>
       </c>
       <c r="G78" s="30"/>
       <c r="H78" s="10"/>
     </row>
     <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="B79" s="23" t="s">
         <v>358</v>
-      </c>
-      <c r="B79" s="23" t="s">
-        <v>359</v>
       </c>
       <c r="C79" s="23"/>
       <c r="D79" s="23"/>
       <c r="E79" s="25" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G79" s="37"/>
       <c r="H79" s="10"/>

</xml_diff>